<commit_message>
Fixed Makefile for automotive/bitcount. Added results for automotive/bitcount.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">automotive/basicmath/basicmathlarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automotive/bitcount/bitcnts 100000000</t>
   </si>
 </sst>
 </file>
@@ -137,15 +140,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -189,6 +192,20 @@
       </c>
       <c r="D3" s="0" t="n">
         <v>1.09</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Makefile for automotive/qsort. Added results for automotive/qsort.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">automotive/bitcount/bitcnts 100000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automotive/qsort/qsort_small input_small.dat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automotive/qsort/qsort_large input_large.dat</t>
   </si>
 </sst>
 </file>
@@ -140,15 +146,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -206,6 +212,34 @@
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Makefile for automotive/susan. Added results for automotive/susan.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">command</t>
   </si>
   <si>
     <t xml:space="preserve">time_real</t>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t xml:space="preserve">automotive/qsort/qsort_large input_large.dat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automotive/susan/susan input_large.pgm output_large.smoothing.pgm -s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automotive/susan/susan input_large.pgm output_large.edges.pgm -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automotive/susan/susan input_large.pgm output_large.corners.pgm -c</t>
   </si>
 </sst>
 </file>
@@ -146,15 +155,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="61.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -240,6 +249,48 @@
       </c>
       <c r="D6" s="0" t="n">
         <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed results for automotive/* and consumer/jpeg to runme_large.sh command.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -34,28 +34,19 @@
     <t xml:space="preserve">time_system</t>
   </si>
   <si>
-    <t xml:space="preserve">automotive/basicmath/basicmathsmall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">automotive/basicmath/basicmathlarge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">automotive/bitcount/bitcnts 100000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">automotive/qsort/qsort_small input_small.dat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">automotive/qsort/qsort_large input_large.dat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">automotive/susan/susan input_large.pgm output_large.smoothing.pgm -s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">automotive/susan/susan input_large.pgm output_large.edges.pgm -e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">automotive/susan/susan input_large.pgm output_large.corners.pgm -c</t>
+    <t xml:space="preserve">automotive/basicmath/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automotive/bitcount/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automotive/qsort/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automotive/susan/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumer/jpeg/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -155,10 +146,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -186,13 +177,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>0.01</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0.05</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -200,96 +191,54 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2.68</v>
+        <v>0.06</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>5</v>
+        <v>0.04</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.06</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="n">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0.29</v>
-      </c>
       <c r="C6" s="0" t="n">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added results for consumer/lame.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">consumer/jpeg/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumer/lame/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -146,10 +149,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -242,6 +245,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results for consumer/mad.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">consumer/lame/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumer/mad/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -64,6 +67,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -149,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -259,6 +263,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results for consumer/typeset.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">consumer/mad/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumer/typeset/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
@@ -277,6 +280,20 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results for network/dijkstra.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">consumer/typeset/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">network/dijkstra/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -156,10 +159,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -294,6 +297,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results for office/rsynth.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -61,7 +61,10 @@
     <t xml:space="preserve">network/dijkstra/runme_large.sh</t>
   </si>
   <si>
-    <t xml:space="preserve">network/patricia/runme_small.sh</t>
+    <t xml:space="preserve">network/patricia/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">office/rsynth/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -162,10 +165,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -328,6 +331,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results of office/stringsearch.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">office/rsynth/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">office/stringsearch/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -165,10 +168,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -345,6 +348,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results of security/blowfish.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">office/stringsearch/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">security/blowfish/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -168,10 +171,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,6 +365,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added security/pgp compile and output files to .gitignore.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">security/blowfish/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">security/pgp/runme.sh</t>
   </si>
 </sst>
 </file>
@@ -171,10 +174,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -379,6 +382,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results of security/sha.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">security/pgp/runme.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">security/sha/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -174,10 +177,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,6 +399,20 @@
         <v>0.02</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results of telecomm/CRC32.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">security/sha/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telecomm/CRC32/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -177,10 +180,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -413,6 +416,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results of telecomm/adpcm.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t xml:space="preserve">telecomm/CRC32/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telecomm/FFT/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telecomm/adpcm/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -180,10 +186,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -430,6 +436,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added results of telecomm/gsm.
</commit_message>
<xml_diff>
--- a/results/user_vs_system_time.xlsx
+++ b/results/user_vs_system_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">command</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">telecomm/adpcm/runme_large.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telecomm/gsm/runme_large.sh</t>
   </si>
 </sst>
 </file>
@@ -186,10 +189,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -464,6 +467,20 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>